<commit_message>
BOMs and PDF with schematic
</commit_message>
<xml_diff>
--- a/Project Outputs for Sampling_Scope/BOM/JLCPCB_CPL-Sampling_Scope(JLCPCB).xlsx
+++ b/Project Outputs for Sampling_Scope/BOM/JLCPCB_CPL-Sampling_Scope(JLCPCB).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\SamplingScope\Project Outputs for Sampling_Scope\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D1480FA-BEC1-48DA-80B9-40536DAA0162}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{795B0875-CA39-4487-B2AF-CC0DDFD7F1A6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1380" yWindow="1935" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7200" yWindow="3675" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM-CSMB_MainBoard(L1 Base)" sheetId="1" r:id="rId1"/>
@@ -915,6 +915,12 @@
     <t>C1</t>
   </si>
   <si>
+    <t>Center-X(mm)</t>
+  </si>
+  <si>
+    <t>Center-Y(mm)</t>
+  </si>
+  <si>
     <t>Layer</t>
   </si>
   <si>
@@ -922,12 +928,6 @@
   </si>
   <si>
     <t>Rotation</t>
-  </si>
-  <si>
-    <t>Mid X</t>
-  </si>
-  <si>
-    <t>Mid Y</t>
   </si>
 </sst>
 </file>
@@ -1308,7 +1308,7 @@
   <dimension ref="A1:E370"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1325,16 +1325,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>299</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>295</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1348,7 +1348,7 @@
         <v>76.070999999999998</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E2" s="1">
         <v>180</v>
@@ -1365,7 +1365,7 @@
         <v>75.070999999999998</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E3" s="1">
         <v>180</v>
@@ -1382,7 +1382,7 @@
         <v>81.2</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E4" s="1">
         <v>0</v>
@@ -1399,7 +1399,7 @@
         <v>81.3</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E5" s="1">
         <v>180</v>
@@ -1416,7 +1416,7 @@
         <v>78.3</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E6" s="1">
         <v>270</v>
@@ -1433,7 +1433,7 @@
         <v>93.7</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E7" s="1">
         <v>0</v>
@@ -1450,7 +1450,7 @@
         <v>91</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E8" s="1">
         <v>180</v>
@@ -1467,7 +1467,7 @@
         <v>90</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E9" s="1">
         <v>180</v>
@@ -1484,7 +1484,7 @@
         <v>87.1</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E10" s="1">
         <v>180</v>
@@ -1501,7 +1501,7 @@
         <v>88.6</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E11" s="1">
         <v>0</v>
@@ -1518,7 +1518,7 @@
         <v>93.7</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E12" s="1">
         <v>90</v>
@@ -1535,7 +1535,7 @@
         <v>93.7</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E13" s="1">
         <v>90</v>
@@ -1552,7 +1552,7 @@
         <v>93.7</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E14" s="1">
         <v>90</v>
@@ -1569,7 +1569,7 @@
         <v>93.7</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E15" s="1">
         <v>270</v>
@@ -1586,7 +1586,7 @@
         <v>93.7</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E16" s="1">
         <v>270</v>
@@ -1603,7 +1603,7 @@
         <v>39.524999999999999</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E17" s="1">
         <v>180</v>
@@ -1620,7 +1620,7 @@
         <v>39.524999999999999</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E18" s="1">
         <v>0</v>
@@ -1637,7 +1637,7 @@
         <v>38.524999999999999</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E19" s="1">
         <v>0</v>
@@ -1654,7 +1654,7 @@
         <v>38.524999999999999</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E20" s="1">
         <v>180</v>
@@ -1671,7 +1671,7 @@
         <v>53.5</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E21" s="1">
         <v>180</v>
@@ -1688,7 +1688,7 @@
         <v>53.5</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E22" s="1">
         <v>180</v>
@@ -1705,7 +1705,7 @@
         <v>53.5</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E23" s="1">
         <v>180</v>
@@ -1722,7 +1722,7 @@
         <v>53.5</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E24" s="1">
         <v>180</v>
@@ -1739,7 +1739,7 @@
         <v>54.9</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E25" s="1">
         <v>90</v>
@@ -1756,7 +1756,7 @@
         <v>54.9</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E26" s="1">
         <v>90</v>
@@ -1773,7 +1773,7 @@
         <v>54.9</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E27" s="1">
         <v>90</v>
@@ -1790,7 +1790,7 @@
         <v>54.9</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E28" s="1">
         <v>90</v>
@@ -1807,7 +1807,7 @@
         <v>84.1</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E29" s="1">
         <v>0</v>
@@ -1824,7 +1824,7 @@
         <v>80</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E30" s="1">
         <v>0</v>
@@ -1841,7 +1841,7 @@
         <v>85.3</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E31" s="1">
         <v>0</v>
@@ -1858,7 +1858,7 @@
         <v>72</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E32" s="1">
         <v>0</v>
@@ -1875,7 +1875,7 @@
         <v>67.900000000000006</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E33" s="1">
         <v>270</v>
@@ -1892,7 +1892,7 @@
         <v>67.900000000000006</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E34" s="1">
         <v>270</v>
@@ -1909,7 +1909,7 @@
         <v>67.900000000000006</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E35" s="1">
         <v>270</v>
@@ -1926,7 +1926,7 @@
         <v>67.900000000000006</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E36" s="1">
         <v>270</v>
@@ -1943,7 +1943,7 @@
         <v>74.599999999999994</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E37" s="1">
         <v>90</v>
@@ -1960,7 +1960,7 @@
         <v>74.599999999999994</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E38" s="1">
         <v>90</v>
@@ -1977,7 +1977,7 @@
         <v>74.599999999999994</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E39" s="1">
         <v>90</v>
@@ -1994,7 +1994,7 @@
         <v>61.5</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E40" s="1">
         <v>0</v>
@@ -2011,7 +2011,7 @@
         <v>74.599999999999994</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E41" s="1">
         <v>90</v>
@@ -2028,7 +2028,7 @@
         <v>62.5</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E42" s="1">
         <v>0</v>
@@ -2045,7 +2045,7 @@
         <v>74.599999999999994</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E43" s="1">
         <v>90</v>
@@ -2062,7 +2062,7 @@
         <v>63.5</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E44" s="1">
         <v>0</v>
@@ -2079,7 +2079,7 @@
         <v>74.599999999999994</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E45" s="1">
         <v>90</v>
@@ -2096,7 +2096,7 @@
         <v>64.5</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E46" s="1">
         <v>0</v>
@@ -2113,7 +2113,7 @@
         <v>70.3</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E47" s="1">
         <v>270</v>
@@ -2130,7 +2130,7 @@
         <v>65.5</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E48" s="1">
         <v>0</v>
@@ -2147,7 +2147,7 @@
         <v>24.3</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E49" s="1">
         <v>180</v>
@@ -2164,7 +2164,7 @@
         <v>25.3</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E50" s="1">
         <v>180</v>
@@ -2181,7 +2181,7 @@
         <v>16.8</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E51" s="1">
         <v>0</v>
@@ -2198,7 +2198,7 @@
         <v>26.3</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E52" s="1">
         <v>180</v>
@@ -2215,7 +2215,7 @@
         <v>27.3</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E53" s="1">
         <v>180</v>
@@ -2232,7 +2232,7 @@
         <v>27.3</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E54" s="1">
         <v>0</v>
@@ -2249,7 +2249,7 @@
         <v>26.3</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E55" s="1">
         <v>0</v>
@@ -2266,7 +2266,7 @@
         <v>23.3</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E56" s="1">
         <v>0</v>
@@ -2283,7 +2283,7 @@
         <v>25.3</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E57" s="1">
         <v>0</v>
@@ -2300,7 +2300,7 @@
         <v>24.3</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E58" s="1">
         <v>0</v>
@@ -2317,7 +2317,7 @@
         <v>25.1</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E59" s="1">
         <v>0</v>
@@ -2334,7 +2334,7 @@
         <v>24.1</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E60" s="1">
         <v>180</v>
@@ -2351,7 +2351,7 @@
         <v>29.5</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E61" s="1">
         <v>270</v>
@@ -2368,7 +2368,7 @@
         <v>27.7</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E62" s="1">
         <v>90</v>
@@ -2385,7 +2385,7 @@
         <v>24.1</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E63" s="1">
         <v>180</v>
@@ -2402,7 +2402,7 @@
         <v>25.1</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E64" s="1">
         <v>0</v>
@@ -2419,7 +2419,7 @@
         <v>29.5</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E65" s="1">
         <v>90</v>
@@ -2436,7 +2436,7 @@
         <v>27.7</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E66" s="1">
         <v>270</v>
@@ -2453,7 +2453,7 @@
         <v>14.4</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E67" s="1">
         <v>90</v>
@@ -2470,7 +2470,7 @@
         <v>26.7</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E68" s="1">
         <v>90</v>
@@ -2487,7 +2487,7 @@
         <v>14.4</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E69" s="1">
         <v>90</v>
@@ -2504,7 +2504,7 @@
         <v>26.7</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E70" s="1">
         <v>90</v>
@@ -2521,7 +2521,7 @@
         <v>25.05</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E71" s="1">
         <v>270</v>
@@ -2538,7 +2538,7 @@
         <v>33.049999999999997</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E72" s="1">
         <v>180</v>
@@ -2555,7 +2555,7 @@
         <v>27.55</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E73" s="1">
         <v>0</v>
@@ -2572,7 +2572,7 @@
         <v>30.25</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E74" s="1">
         <v>270</v>
@@ -2589,7 +2589,7 @@
         <v>27.55</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E75" s="1">
         <v>180</v>
@@ -2606,7 +2606,7 @@
         <v>28.45</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E76" s="1">
         <v>90</v>
@@ -2623,7 +2623,7 @@
         <v>28.55</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E77" s="1">
         <v>180</v>
@@ -2640,7 +2640,7 @@
         <v>30.25</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E78" s="1">
         <v>90</v>
@@ -2657,7 +2657,7 @@
         <v>28.55</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E79" s="1">
         <v>0</v>
@@ -2674,7 +2674,7 @@
         <v>28.45</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E80" s="1">
         <v>270</v>
@@ -2691,7 +2691,7 @@
         <v>14.5</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E81" s="1">
         <v>180</v>
@@ -2708,7 +2708,7 @@
         <v>18.399999999999999</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E82" s="1">
         <v>0</v>
@@ -2725,7 +2725,7 @@
         <v>18.399999999999999</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E83" s="1">
         <v>180</v>
@@ -2742,7 +2742,7 @@
         <v>17.399999999999999</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E84" s="1">
         <v>180</v>
@@ -2759,7 +2759,7 @@
         <v>17.399999999999999</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E85" s="1">
         <v>0</v>
@@ -2776,7 +2776,7 @@
         <v>12.5</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E86" s="1">
         <v>0</v>
@@ -2793,7 +2793,7 @@
         <v>14.5</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E87" s="1">
         <v>180</v>
@@ -2810,7 +2810,7 @@
         <v>94.9</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E88" s="1">
         <v>90</v>
@@ -2827,7 +2827,7 @@
         <v>93.1</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E89" s="1">
         <v>270</v>
@@ -2844,7 +2844,7 @@
         <v>83</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E90" s="1">
         <v>270</v>
@@ -2861,7 +2861,7 @@
         <v>86.2</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E91" s="1">
         <v>90</v>
@@ -2878,7 +2878,7 @@
         <v>86</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E92" s="1">
         <v>270</v>
@@ -2895,7 +2895,7 @@
         <v>83.2</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E93" s="1">
         <v>90</v>
@@ -2912,7 +2912,7 @@
         <v>90</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E94" s="1">
         <v>180</v>
@@ -2929,7 +2929,7 @@
         <v>63.3</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E95" s="1">
         <v>90</v>
@@ -2946,7 +2946,7 @@
         <v>57.1</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E96" s="1">
         <v>180</v>
@@ -2963,7 +2963,7 @@
         <v>72.8</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E97" s="1">
         <v>90</v>
@@ -2980,7 +2980,7 @@
         <v>22.7</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E98" s="1">
         <v>90</v>
@@ -2997,7 +2997,7 @@
         <v>34.700000000000003</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E99" s="1">
         <v>90</v>
@@ -3014,7 +3014,7 @@
         <v>42.6</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E100" s="1">
         <v>90</v>
@@ -3031,7 +3031,7 @@
         <v>42.5</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E101" s="1">
         <v>90</v>
@@ -3048,7 +3048,7 @@
         <v>19.100000000000001</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E102" s="1">
         <v>270</v>
@@ -3065,7 +3065,7 @@
         <v>30.5</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E103" s="1">
         <v>270</v>
@@ -3082,7 +3082,7 @@
         <v>40.799999999999997</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E104" s="1">
         <v>270</v>
@@ -3099,7 +3099,7 @@
         <v>40.700000000000003</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E105" s="1">
         <v>270</v>
@@ -3116,7 +3116,7 @@
         <v>22.7</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E106" s="1">
         <v>270</v>
@@ -3133,7 +3133,7 @@
         <v>34.700000000000003</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E107" s="1">
         <v>270</v>
@@ -3150,7 +3150,7 @@
         <v>40.799999999999997</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E108" s="1">
         <v>90</v>
@@ -3167,7 +3167,7 @@
         <v>40.700000000000003</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E109" s="1">
         <v>90</v>
@@ -3184,7 +3184,7 @@
         <v>15.9</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E110" s="1">
         <v>270</v>
@@ -3201,7 +3201,7 @@
         <v>15.997</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E111" s="1">
         <v>270</v>
@@ -3218,7 +3218,7 @@
         <v>19.547000000000001</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E112" s="1">
         <v>180</v>
@@ -3235,7 +3235,7 @@
         <v>19.547000000000001</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E113" s="1">
         <v>180</v>
@@ -3252,7 +3252,7 @@
         <v>19.547000000000001</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E114" s="1">
         <v>0</v>
@@ -3269,7 +3269,7 @@
         <v>19.547000000000001</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E115" s="1">
         <v>0</v>
@@ -3286,7 +3286,7 @@
         <v>20.547000000000001</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E116" s="1">
         <v>0</v>
@@ -3303,7 +3303,7 @@
         <v>20.547000000000001</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E117" s="1">
         <v>0</v>
@@ -3320,7 +3320,7 @@
         <v>20.547000000000001</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E118" s="1">
         <v>180</v>
@@ -3337,7 +3337,7 @@
         <v>20.547000000000001</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E119" s="1">
         <v>180</v>
@@ -3354,7 +3354,7 @@
         <v>52.347999999999999</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E120" s="1">
         <v>180</v>
@@ -3371,7 +3371,7 @@
         <v>61.55</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E121" s="1">
         <v>270</v>
@@ -3388,7 +3388,7 @@
         <v>15.047000000000001</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E122" s="1">
         <v>90</v>
@@ -3405,7 +3405,7 @@
         <v>14.997</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E123" s="1">
         <v>90</v>
@@ -3422,7 +3422,7 @@
         <v>17.047000000000001</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E124" s="1">
         <v>270</v>
@@ -3439,7 +3439,7 @@
         <v>17.047000000000001</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E125" s="1">
         <v>270</v>
@@ -3456,7 +3456,7 @@
         <v>19.297000000000001</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E126" s="1">
         <v>90</v>
@@ -3473,7 +3473,7 @@
         <v>19.297000000000001</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E127" s="1">
         <v>90</v>
@@ -3490,7 +3490,7 @@
         <v>19.297000000000001</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E128" s="1">
         <v>90</v>
@@ -3507,7 +3507,7 @@
         <v>19.297000000000001</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E129" s="1">
         <v>90</v>
@@ -3524,7 +3524,7 @@
         <v>15.047000000000001</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E130" s="1">
         <v>270</v>
@@ -3541,7 +3541,7 @@
         <v>15.047000000000001</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E131" s="1">
         <v>270</v>
@@ -3558,7 +3558,7 @@
         <v>17.047000000000001</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E132" s="1">
         <v>90</v>
@@ -3575,7 +3575,7 @@
         <v>17.047000000000001</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E133" s="1">
         <v>90</v>
@@ -3592,7 +3592,7 @@
         <v>31.9</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E134" s="1">
         <v>0</v>
@@ -3609,7 +3609,7 @@
         <v>31.9</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E135" s="1">
         <v>180</v>
@@ -3626,7 +3626,7 @@
         <v>32.9</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E136" s="1">
         <v>180</v>
@@ -3643,7 +3643,7 @@
         <v>32.9</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E137" s="1">
         <v>0</v>
@@ -3660,7 +3660,7 @@
         <v>79.099999999999994</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E138" s="1">
         <v>90</v>
@@ -3677,7 +3677,7 @@
         <v>53</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E139" s="1">
         <v>180</v>
@@ -3694,7 +3694,7 @@
         <v>77.900000000000006</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E140" s="1">
         <v>0</v>
@@ -3711,7 +3711,7 @@
         <v>77.900000000000006</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E141" s="1">
         <v>0</v>
@@ -3728,7 +3728,7 @@
         <v>52.9</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E142" s="1">
         <v>0</v>
@@ -3745,7 +3745,7 @@
         <v>67.400000000000006</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E143" s="1">
         <v>270</v>
@@ -3762,7 +3762,7 @@
         <v>15.5</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E144" s="1">
         <v>0</v>
@@ -3779,7 +3779,7 @@
         <v>23.1</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E145" s="1">
         <v>180</v>
@@ -3796,7 +3796,7 @@
         <v>97</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E146" s="1">
         <v>0</v>
@@ -3813,7 +3813,7 @@
         <v>87.6</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E147" s="1">
         <v>180</v>
@@ -3830,7 +3830,7 @@
         <v>89.6</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E148" s="1">
         <v>180</v>
@@ -3847,7 +3847,7 @@
         <v>93.7</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E149" s="1">
         <v>90</v>
@@ -3864,7 +3864,7 @@
         <v>37</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E150" s="1">
         <v>90</v>
@@ -3881,7 +3881,7 @@
         <v>37</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E151" s="1">
         <v>90</v>
@@ -3898,7 +3898,7 @@
         <v>54.9</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E152" s="1">
         <v>90</v>
@@ -3915,7 +3915,7 @@
         <v>54.9</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E153" s="1">
         <v>90</v>
@@ -3932,7 +3932,7 @@
         <v>54.9</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E154" s="1">
         <v>90</v>
@@ -3949,7 +3949,7 @@
         <v>54.9</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E155" s="1">
         <v>90</v>
@@ -3966,7 +3966,7 @@
         <v>54.9</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E156" s="1">
         <v>90</v>
@@ -3983,7 +3983,7 @@
         <v>54.9</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E157" s="1">
         <v>90</v>
@@ -4000,7 +4000,7 @@
         <v>54.9</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E158" s="1">
         <v>90</v>
@@ -4017,7 +4017,7 @@
         <v>54.9</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E159" s="1">
         <v>90</v>
@@ -4034,7 +4034,7 @@
         <v>80</v>
       </c>
       <c r="D160" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E160" s="1">
         <v>180</v>
@@ -4051,7 +4051,7 @@
         <v>80.7</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E161" s="1">
         <v>0</v>
@@ -4068,7 +4068,7 @@
         <v>80</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E162" s="1">
         <v>0</v>
@@ -4085,7 +4085,7 @@
         <v>80.8</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E163" s="1">
         <v>180</v>
@@ -4102,7 +4102,7 @@
         <v>82.6</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E164" s="1">
         <v>180</v>
@@ -4119,7 +4119,7 @@
         <v>79</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E165" s="1">
         <v>180</v>
@@ -4136,7 +4136,7 @@
         <v>71</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E166" s="1">
         <v>0</v>
@@ -4153,7 +4153,7 @@
         <v>66.5</v>
       </c>
       <c r="D167" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E167" s="1">
         <v>180</v>
@@ -4170,7 +4170,7 @@
         <v>71.400000000000006</v>
       </c>
       <c r="D168" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E168" s="1">
         <v>90</v>
@@ -4187,7 +4187,7 @@
         <v>15.6</v>
       </c>
       <c r="D169" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E169" s="1">
         <v>180</v>
@@ -4204,7 +4204,7 @@
         <v>22.4</v>
       </c>
       <c r="D170" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E170" s="1">
         <v>0</v>
@@ -4221,7 +4221,7 @@
         <v>24.5</v>
       </c>
       <c r="D171" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E171" s="1">
         <v>90</v>
@@ -4238,7 +4238,7 @@
         <v>32.299999999999997</v>
       </c>
       <c r="D172" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E172" s="1">
         <v>90</v>
@@ -4255,7 +4255,7 @@
         <v>24.5</v>
       </c>
       <c r="D173" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E173" s="1">
         <v>90</v>
@@ -4272,7 +4272,7 @@
         <v>32.299999999999997</v>
       </c>
       <c r="D174" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E174" s="1">
         <v>90</v>
@@ -4289,7 +4289,7 @@
         <v>14.4</v>
       </c>
       <c r="D175" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E175" s="1">
         <v>90</v>
@@ -4306,7 +4306,7 @@
         <v>26.7</v>
       </c>
       <c r="D176" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E176" s="1">
         <v>90</v>
@@ -4323,7 +4323,7 @@
         <v>14.8</v>
       </c>
       <c r="D177" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E177" s="1">
         <v>180</v>
@@ -4340,7 +4340,7 @@
         <v>27.2</v>
       </c>
       <c r="D178" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E178" s="1">
         <v>180</v>
@@ -4357,7 +4357,7 @@
         <v>19.100000000000001</v>
       </c>
       <c r="D179" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E179" s="1">
         <v>90</v>
@@ -4374,7 +4374,7 @@
         <v>31</v>
       </c>
       <c r="D180" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E180" s="1">
         <v>270</v>
@@ -4391,7 +4391,7 @@
         <v>19.8</v>
       </c>
       <c r="D181" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E181" s="1">
         <v>0</v>
@@ -4408,7 +4408,7 @@
         <v>31.6</v>
       </c>
       <c r="D182" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E182" s="1">
         <v>90</v>
@@ -4425,7 +4425,7 @@
         <v>23.15</v>
       </c>
       <c r="D183" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E183" s="1">
         <v>270</v>
@@ -4442,7 +4442,7 @@
         <v>33.049999999999997</v>
       </c>
       <c r="D184" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E184" s="1">
         <v>180</v>
@@ -4459,7 +4459,7 @@
         <v>12.5</v>
       </c>
       <c r="D185" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E185" s="1">
         <v>0</v>
@@ -4476,7 +4476,7 @@
         <v>13.1</v>
       </c>
       <c r="D186" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E186" s="1">
         <v>270</v>
@@ -4493,7 +4493,7 @@
         <v>13.5</v>
       </c>
       <c r="D187" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E187" s="1">
         <v>180</v>
@@ -4510,7 +4510,7 @@
         <v>15.5</v>
       </c>
       <c r="D188" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E188" s="1">
         <v>0</v>
@@ -4527,7 +4527,7 @@
         <v>13.5</v>
       </c>
       <c r="D189" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E189" s="1">
         <v>180</v>
@@ -4544,7 +4544,7 @@
         <v>87.724999999999994</v>
       </c>
       <c r="D190" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E190" s="1">
         <v>90</v>
@@ -4561,7 +4561,7 @@
         <v>87.2</v>
       </c>
       <c r="D191" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E191" s="1">
         <v>0</v>
@@ -4578,7 +4578,7 @@
         <v>89</v>
       </c>
       <c r="D192" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E192" s="1">
         <v>0</v>
@@ -4595,7 +4595,7 @@
         <v>90.8</v>
       </c>
       <c r="D193" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E193" s="1">
         <v>0</v>
@@ -4612,7 +4612,7 @@
         <v>87.7</v>
       </c>
       <c r="D194" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E194" s="1">
         <v>270</v>
@@ -4629,7 +4629,7 @@
         <v>90.825000000000003</v>
       </c>
       <c r="D195" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E195" s="1">
         <v>270</v>
@@ -4646,7 +4646,7 @@
         <v>95.224999999999994</v>
       </c>
       <c r="D196" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E196" s="1">
         <v>90</v>
@@ -4663,7 +4663,7 @@
         <v>94.2</v>
       </c>
       <c r="D197" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E197" s="1">
         <v>90</v>
@@ -4680,7 +4680,7 @@
         <v>90.7</v>
       </c>
       <c r="D198" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E198" s="1">
         <v>270</v>
@@ -4697,7 +4697,7 @@
         <v>90.7</v>
       </c>
       <c r="D199" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E199" s="1">
         <v>270</v>
@@ -4714,7 +4714,7 @@
         <v>94.2</v>
       </c>
       <c r="D200" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E200" s="1">
         <v>90</v>
@@ -4731,7 +4731,7 @@
         <v>94.2</v>
       </c>
       <c r="D201" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E201" s="1">
         <v>90</v>
@@ -4748,7 +4748,7 @@
         <v>93.325000000000003</v>
       </c>
       <c r="D202" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E202" s="1">
         <v>90</v>
@@ -4765,7 +4765,7 @@
         <v>95.224999999999994</v>
       </c>
       <c r="D203" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E203" s="1">
         <v>0</v>
@@ -4782,7 +4782,7 @@
         <v>89.4</v>
       </c>
       <c r="D204" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E204" s="1">
         <v>270</v>
@@ -4799,7 +4799,7 @@
         <v>89.4</v>
       </c>
       <c r="D205" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E205" s="1">
         <v>270</v>
@@ -4816,7 +4816,7 @@
         <v>89.4</v>
       </c>
       <c r="D206" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E206" s="1">
         <v>270</v>
@@ -4833,7 +4833,7 @@
         <v>90.6</v>
       </c>
       <c r="D207" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E207" s="1">
         <v>180</v>
@@ -4850,7 +4850,7 @@
         <v>97.2</v>
       </c>
       <c r="D208" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E208" s="1">
         <v>90</v>
@@ -4867,7 +4867,7 @@
         <v>97.2</v>
       </c>
       <c r="D209" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E209" s="1">
         <v>90</v>
@@ -4884,7 +4884,7 @@
         <v>91.2</v>
       </c>
       <c r="D210" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E210" s="1">
         <v>0</v>
@@ -4901,7 +4901,7 @@
         <v>82.2</v>
       </c>
       <c r="D211" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E211" s="1">
         <v>270</v>
@@ -4918,7 +4918,7 @@
         <v>87.2</v>
       </c>
       <c r="D212" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E212" s="1">
         <v>90</v>
@@ -4935,7 +4935,7 @@
         <v>86.8</v>
       </c>
       <c r="D213" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E213" s="1">
         <v>90</v>
@@ -4952,7 +4952,7 @@
         <v>87.2</v>
       </c>
       <c r="D214" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E214" s="1">
         <v>90</v>
@@ -4969,7 +4969,7 @@
         <v>84.5</v>
       </c>
       <c r="D215" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E215" s="1">
         <v>0</v>
@@ -4986,7 +4986,7 @@
         <v>84.7</v>
       </c>
       <c r="D216" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E216" s="1">
         <v>180</v>
@@ -5003,7 +5003,7 @@
         <v>84.6</v>
       </c>
       <c r="D217" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E217" s="1">
         <v>0</v>
@@ -5020,7 +5020,7 @@
         <v>84.6</v>
       </c>
       <c r="D218" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E218" s="1">
         <v>180</v>
@@ -5037,7 +5037,7 @@
         <v>86.1</v>
       </c>
       <c r="D219" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E219" s="1">
         <v>0</v>
@@ -5054,7 +5054,7 @@
         <v>83.1</v>
       </c>
       <c r="D220" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E220" s="1">
         <v>180</v>
@@ -5071,7 +5071,7 @@
         <v>83.1</v>
       </c>
       <c r="D221" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E221" s="1">
         <v>0</v>
@@ -5088,7 +5088,7 @@
         <v>86.1</v>
       </c>
       <c r="D222" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E222" s="1">
         <v>180</v>
@@ -5105,7 +5105,7 @@
         <v>82.5</v>
       </c>
       <c r="D223" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E223" s="1">
         <v>90</v>
@@ -5122,7 +5122,7 @@
         <v>81.400000000000006</v>
       </c>
       <c r="D224" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E224" s="1">
         <v>180</v>
@@ -5139,7 +5139,7 @@
         <v>52.6</v>
       </c>
       <c r="D225" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E225" s="1">
         <v>270</v>
@@ -5156,7 +5156,7 @@
         <v>72.5</v>
       </c>
       <c r="D226" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E226" s="1">
         <v>0</v>
@@ -5173,7 +5173,7 @@
         <v>58.1</v>
       </c>
       <c r="D227" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E227" s="1">
         <v>180</v>
@@ -5190,7 +5190,7 @@
         <v>56.1</v>
       </c>
       <c r="D228" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E228" s="1">
         <v>180</v>
@@ -5207,7 +5207,7 @@
         <v>55.1</v>
       </c>
       <c r="D229" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E229" s="1">
         <v>180</v>
@@ -5224,7 +5224,7 @@
         <v>54.1</v>
       </c>
       <c r="D230" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E230" s="1">
         <v>180</v>
@@ -5241,7 +5241,7 @@
         <v>54.1</v>
       </c>
       <c r="D231" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E231" s="1">
         <v>0</v>
@@ -5258,7 +5258,7 @@
         <v>72.8</v>
       </c>
       <c r="D232" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E232" s="1">
         <v>90</v>
@@ -5275,7 +5275,7 @@
         <v>53</v>
       </c>
       <c r="D233" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E233" s="1">
         <v>180</v>
@@ -5292,7 +5292,7 @@
         <v>66.400000000000006</v>
       </c>
       <c r="D234" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E234" s="1">
         <v>90</v>
@@ -5309,7 +5309,7 @@
         <v>59.4</v>
       </c>
       <c r="D235" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E235" s="1">
         <v>270</v>
@@ -5326,7 +5326,7 @@
         <v>78</v>
       </c>
       <c r="D236" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E236" s="1">
         <v>180</v>
@@ -5343,7 +5343,7 @@
         <v>73.900000000000006</v>
       </c>
       <c r="D237" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E237" s="1">
         <v>270</v>
@@ -5360,7 +5360,7 @@
         <v>61.9</v>
       </c>
       <c r="D238" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E238" s="1">
         <v>270</v>
@@ -5377,7 +5377,7 @@
         <v>53</v>
       </c>
       <c r="D239" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E239" s="1">
         <v>180</v>
@@ -5394,7 +5394,7 @@
         <v>20.9</v>
       </c>
       <c r="D240" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E240" s="1">
         <v>270</v>
@@ -5411,7 +5411,7 @@
         <v>32.9</v>
       </c>
       <c r="D241" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E241" s="1">
         <v>270</v>
@@ -5428,7 +5428,7 @@
         <v>42.6</v>
       </c>
       <c r="D242" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E242" s="1">
         <v>90</v>
@@ -5445,7 +5445,7 @@
         <v>42.5</v>
       </c>
       <c r="D243" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E243" s="1">
         <v>90</v>
@@ -5462,7 +5462,7 @@
         <v>22.4</v>
       </c>
       <c r="D244" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E244" s="1">
         <v>0</v>
@@ -5479,7 +5479,7 @@
         <v>34.299999999999997</v>
       </c>
       <c r="D245" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E245" s="1">
         <v>0</v>
@@ -5496,7 +5496,7 @@
         <v>40.299999999999997</v>
       </c>
       <c r="D246" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E246" s="1">
         <v>0</v>
@@ -5513,7 +5513,7 @@
         <v>40.700000000000003</v>
       </c>
       <c r="D247" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E247" s="1">
         <v>0</v>
@@ -5530,7 +5530,7 @@
         <v>23.3</v>
       </c>
       <c r="D248" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E248" s="1">
         <v>0</v>
@@ -5547,7 +5547,7 @@
         <v>35.4</v>
       </c>
       <c r="D249" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E249" s="1">
         <v>0</v>
@@ -5564,7 +5564,7 @@
         <v>41.4</v>
       </c>
       <c r="D250" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E250" s="1">
         <v>0</v>
@@ -5581,7 +5581,7 @@
         <v>41.7</v>
       </c>
       <c r="D251" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E251" s="1">
         <v>0</v>
@@ -5598,7 +5598,7 @@
         <v>30.6</v>
       </c>
       <c r="D252" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E252" s="1">
         <v>90</v>
@@ -5615,7 +5615,7 @@
         <v>42</v>
       </c>
       <c r="D253" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E253" s="1">
         <v>90</v>
@@ -5632,7 +5632,7 @@
         <v>48.7</v>
       </c>
       <c r="D254" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E254" s="1">
         <v>90</v>
@@ -5649,7 +5649,7 @@
         <v>48.6</v>
       </c>
       <c r="D255" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E255" s="1">
         <v>90</v>
@@ -5666,7 +5666,7 @@
         <v>28.4</v>
       </c>
       <c r="D256" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E256" s="1">
         <v>0</v>
@@ -5683,7 +5683,7 @@
         <v>40.4</v>
       </c>
       <c r="D257" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E257" s="1">
         <v>0</v>
@@ -5700,7 +5700,7 @@
         <v>45.9</v>
       </c>
       <c r="D258" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E258" s="1">
         <v>0</v>
@@ -5717,7 +5717,7 @@
         <v>46.2</v>
       </c>
       <c r="D259" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E259" s="1">
         <v>0</v>
@@ -5734,7 +5734,7 @@
         <v>31</v>
       </c>
       <c r="D260" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E260" s="1">
         <v>270</v>
@@ -5751,7 +5751,7 @@
         <v>43.3</v>
       </c>
       <c r="D261" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E261" s="1">
         <v>0</v>
@@ -5768,7 +5768,7 @@
         <v>48.4</v>
       </c>
       <c r="D262" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E262" s="1">
         <v>270</v>
@@ -5785,7 +5785,7 @@
         <v>48.6</v>
       </c>
       <c r="D263" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E263" s="1">
         <v>90</v>
@@ -5802,7 +5802,7 @@
         <v>29.4</v>
       </c>
       <c r="D264" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E264" s="1">
         <v>0</v>
@@ -5819,7 +5819,7 @@
         <v>41.4</v>
       </c>
       <c r="D265" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E265" s="1">
         <v>0</v>
@@ -5836,7 +5836,7 @@
         <v>47</v>
       </c>
       <c r="D266" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E266" s="1">
         <v>0</v>
@@ -5853,7 +5853,7 @@
         <v>47.2</v>
       </c>
       <c r="D267" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E267" s="1">
         <v>0</v>
@@ -5870,7 +5870,7 @@
         <v>57.7</v>
       </c>
       <c r="D268" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E268" s="1">
         <v>180</v>
@@ -5887,7 +5887,7 @@
         <v>58.7</v>
       </c>
       <c r="D269" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E269" s="1">
         <v>0</v>
@@ -5904,7 +5904,7 @@
         <v>61.2</v>
       </c>
       <c r="D270" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E270" s="1">
         <v>270</v>
@@ -5921,7 +5921,7 @@
         <v>58.7</v>
       </c>
       <c r="D271" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E271" s="1">
         <v>180</v>
@@ -5938,7 +5938,7 @@
         <v>18.5</v>
       </c>
       <c r="D272" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E272" s="1">
         <v>0</v>
@@ -5955,7 +5955,7 @@
         <v>18.497</v>
       </c>
       <c r="D273" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E273" s="1">
         <v>0</v>
@@ -5972,7 +5972,7 @@
         <v>18.5</v>
       </c>
       <c r="D274" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E274" s="1">
         <v>180</v>
@@ -5989,7 +5989,7 @@
         <v>18.497</v>
       </c>
       <c r="D275" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E275" s="1">
         <v>180</v>
@@ -6006,7 +6006,7 @@
         <v>14.4</v>
       </c>
       <c r="D276" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E276" s="1">
         <v>270</v>
@@ -6023,7 +6023,7 @@
         <v>14.397</v>
       </c>
       <c r="D277" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E277" s="1">
         <v>270</v>
@@ -6040,7 +6040,7 @@
         <v>15.9</v>
       </c>
       <c r="D278" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E278" s="1">
         <v>90</v>
@@ -6057,7 +6057,7 @@
         <v>15.997</v>
       </c>
       <c r="D279" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E279" s="1">
         <v>90</v>
@@ -6074,7 +6074,7 @@
         <v>52.9</v>
       </c>
       <c r="D280" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E280" s="1">
         <v>180</v>
@@ -6091,7 +6091,7 @@
         <v>59.5</v>
       </c>
       <c r="D281" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E281" s="1">
         <v>270</v>
@@ -6108,7 +6108,7 @@
         <v>54.347000000000001</v>
       </c>
       <c r="D282" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E282" s="1">
         <v>90</v>
@@ -6125,7 +6125,7 @@
         <v>58.8</v>
       </c>
       <c r="D283" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E283" s="1">
         <v>180</v>
@@ -6142,7 +6142,7 @@
         <v>13</v>
       </c>
       <c r="D284" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E284" s="1">
         <v>0</v>
@@ -6159,7 +6159,7 @@
         <v>12.997</v>
       </c>
       <c r="D285" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E285" s="1">
         <v>0</v>
@@ -6176,7 +6176,7 @@
         <v>23</v>
       </c>
       <c r="D286" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E286" s="1">
         <v>270</v>
@@ -6193,7 +6193,7 @@
         <v>22.997</v>
       </c>
       <c r="D287" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E287" s="1">
         <v>270</v>
@@ -6210,7 +6210,7 @@
         <v>24.7</v>
       </c>
       <c r="D288" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E288" s="1">
         <v>0</v>
@@ -6227,7 +6227,7 @@
         <v>24.797000000000001</v>
       </c>
       <c r="D289" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E289" s="1">
         <v>0</v>
@@ -6244,7 +6244,7 @@
         <v>19.297000000000001</v>
       </c>
       <c r="D290" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E290" s="1">
         <v>270</v>
@@ -6261,7 +6261,7 @@
         <v>19.297000000000001</v>
       </c>
       <c r="D291" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E291" s="1">
         <v>270</v>
@@ -6278,7 +6278,7 @@
         <v>89.6</v>
       </c>
       <c r="D292" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E292" s="1">
         <v>90</v>
@@ -6295,7 +6295,7 @@
         <v>34.9</v>
       </c>
       <c r="D293" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E293" s="1">
         <v>270</v>
@@ -6312,7 +6312,7 @@
         <v>43.3</v>
       </c>
       <c r="D294" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E294" s="1">
         <v>0</v>
@@ -6329,7 +6329,7 @@
         <v>43.3</v>
       </c>
       <c r="D295" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E295" s="1">
         <v>180</v>
@@ -6868,6 +6868,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D5F7C78E3414E24A91C2703725BF92FC" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1c4adfc77660b6ce239d14e1c7862ad9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f6772ea1-6e7c-4f6d-98c0-66ca2514fea8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="645695edfd6e67b10d59853d0d05d811" ns2:_="">
     <xsd:import namespace="f6772ea1-6e7c-4f6d-98c0-66ca2514fea8"/>
@@ -6999,15 +7008,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -7015,6 +7015,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C52FC9F2-0211-4826-991F-C9BB213F71B5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6217E9EE-715F-4310-AA61-C9A633A15441}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7028,14 +7036,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C52FC9F2-0211-4826-991F-C9BB213F71B5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>